<commit_message>
feat: add phys lab 3
</commit_message>
<xml_diff>
--- a/2 year/Физика/Лабораторная работа 3.03/Данные.xlsx
+++ b/2 year/Физика/Лабораторная работа 3.03/Данные.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azat2\itmo\2 year\Физика\Лабораторная работа 3.03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35123E1E-824B-4788-8994-BABFB96C567B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2CA69A-2105-4185-8C8E-A9E0005E323D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>N опыта</t>
   </si>
@@ -85,6 +85,9 @@
   <si>
     <t>I_a / I_L</t>
   </si>
+  <si>
+    <t>I_кр</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -372,11 +375,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -419,6 +431,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -512,7 +534,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10419743401785832"/>
+          <c:y val="0.13667385009272257"/>
+          <c:w val="0.79284399742182055"/>
+          <c:h val="0.65438327648318062"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -532,23 +564,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Лист1!$E$5:$E$25</c:f>
@@ -713,23 +730,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Лист1!$E$5:$E$25</c:f>
@@ -884,7 +886,7 @@
         <c:dLbls>
           <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -895,6 +897,153 @@
         <c:axId val="1419261551"/>
         <c:axId val="1419258191"/>
       </c:lineChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>I_кр</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-40CF-496B-B545-7AF83C76F6E8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$H$5:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="9">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-40CF-496B-B545-7AF83C76F6E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>I_кр</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$G$5:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="9">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-40CF-496B-B545-7AF83C76F6E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1419261551"/>
+        <c:axId val="1419258191"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="1419261551"/>
         <c:scaling>
@@ -1410,7 +1559,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$K$6:$K$25</c:f>
+              <c:f>Лист1!$L$6:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1479,7 +1628,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$J$6:$J$24</c:f>
+              <c:f>Лист1!$K$6:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1582,7 +1731,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$K$6:$K$25</c:f>
+              <c:f>Лист1!$L$6:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1651,7 +1800,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$L$6:$L$25</c:f>
+              <c:f>Лист1!$M$6:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3161,7 +3310,7 @@
       <xdr:rowOff>150551</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>361504</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>51657</xdr:rowOff>
@@ -3191,13 +3340,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>331304</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>122582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>530087</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>82826</xdr:rowOff>
@@ -3491,20 +3640,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:S25"/>
+  <dimension ref="B1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
@@ -3514,30 +3663,31 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="25"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="24"/>
       <c r="K2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="P2" s="17" t="s">
+      <c r="L2" s="24"/>
+      <c r="M2" s="25"/>
+      <c r="Q2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="R2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="S2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B3" s="22"/>
       <c r="C3" s="26" t="s">
         <v>3</v>
@@ -3547,31 +3697,32 @@
         <v>4</v>
       </c>
       <c r="F3" s="27"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="26" t="s">
+      <c r="G3" s="31"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="26"/>
+      <c r="L3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="P3" s="4">
+      <c r="M3" s="27"/>
+      <c r="Q3" s="4">
         <v>9</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>0.22</v>
       </c>
-      <c r="R3" s="2">
-        <f>$Q$8*Q3*$Q$10/(SQRT($Q$6^2 + $Q$7^2))</f>
+      <c r="S3" s="2">
+        <f>$R$8*R3*$R$10/(SQRT($R$6^2 + $R$7^2))</f>
         <v>8.0329524684307659E-3</v>
       </c>
-      <c r="S3" s="3">
-        <f>(8*P3)/(R3^2*$Q$9^2)</f>
+      <c r="T3" s="3">
+        <f>(8*Q3)/(S3^2*$R$9^2)</f>
         <v>123976563088.53537</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="23"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -3585,35 +3736,41 @@
       <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="19" t="s">
+      <c r="G4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="L4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="M4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="5">
         <v>11</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4" s="6">
         <v>0.22</v>
       </c>
-      <c r="R4" s="2">
-        <f>$Q$8*Q4*$Q$10/(SQRT($Q$6^2 + $Q$7^2))</f>
+      <c r="S4" s="2">
+        <f>$R$8*R4*$R$10/(SQRT($R$6^2 + $R$7^2))</f>
         <v>8.0329524684307659E-3</v>
       </c>
-      <c r="S4" s="3">
-        <f>(8*P4)/(R4^2*$Q$9^2)</f>
+      <c r="T4" s="3">
+        <f>(8*Q4)/(S4^2*$R$9^2)</f>
         <v>151526910441.54324</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -3629,15 +3786,16 @@
       <c r="F5" s="8">
         <v>0.28010000000000002</v>
       </c>
-      <c r="H5" s="9">
+      <c r="G5" s="33"/>
+      <c r="I5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
         <v>2</v>
       </c>
@@ -3653,33 +3811,34 @@
       <c r="F6" s="3">
         <v>0.2797</v>
       </c>
-      <c r="H6" s="10">
+      <c r="G6" s="33"/>
+      <c r="I6" s="10">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
-        <f t="shared" ref="I6:I24" si="0">C6</f>
+      <c r="J6" s="2">
+        <f t="shared" ref="J6:J24" si="0">C6</f>
         <v>0.03</v>
       </c>
-      <c r="J6" s="2">
-        <f t="shared" ref="J6:J24" si="1">D6/C6</f>
+      <c r="K6" s="2">
+        <f t="shared" ref="K6:K24" si="1">D6/C6</f>
         <v>7.4766666666666666</v>
       </c>
-      <c r="K6" s="2">
-        <f t="shared" ref="K6:K20" si="2">E6</f>
+      <c r="L6" s="2">
+        <f t="shared" ref="L6:L20" si="2">E6</f>
         <v>0.03</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <f>F6/E6</f>
         <v>9.3233333333333341</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="Q6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="R6" s="16">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <v>3</v>
       </c>
@@ -3695,33 +3854,34 @@
       <c r="F7" s="3">
         <v>0.28010000000000002</v>
       </c>
-      <c r="H7" s="10">
+      <c r="G7" s="33"/>
+      <c r="I7" s="10">
         <v>3</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
         <v>4.4819999999999993</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="L7" s="3">
-        <f t="shared" ref="L7:L25" si="3">F7/E7</f>
+      <c r="M7" s="3">
+        <f t="shared" ref="M7:M25" si="3">F7/E7</f>
         <v>5.6020000000000003</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <v>4</v>
       </c>
@@ -3737,34 +3897,35 @@
       <c r="F8" s="3">
         <v>0.28050000000000003</v>
       </c>
-      <c r="H8" s="10">
+      <c r="G8" s="33"/>
+      <c r="I8" s="10">
         <v>4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
         <v>3.198571428571428</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <f t="shared" si="2"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <f t="shared" si="3"/>
         <v>4.0071428571428571</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="R8" s="3">
         <f>4*PI()*10^(-7)</f>
         <v>1.2566370614359173E-6</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
         <v>5</v>
       </c>
@@ -3780,33 +3941,34 @@
       <c r="F9" s="3">
         <v>0.28089999999999998</v>
       </c>
-      <c r="H9" s="10">
+      <c r="G9" s="33"/>
+      <c r="I9" s="10">
         <v>5</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
         <v>2.2429999999999999</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <f t="shared" si="3"/>
         <v>3.1211111111111109</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10">
         <v>6</v>
       </c>
@@ -3822,33 +3984,34 @@
       <c r="F10" s="3">
         <v>0.28110000000000002</v>
       </c>
-      <c r="H10" s="10">
+      <c r="G10" s="33"/>
+      <c r="I10" s="10">
         <v>6</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
         <v>1.726923076923077</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <f t="shared" si="3"/>
         <v>2.3425000000000002</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="R10" s="7">
         <v>1500</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <v>7</v>
       </c>
@@ -3864,27 +4027,28 @@
       <c r="F11" s="3">
         <v>0.28199999999999997</v>
       </c>
-      <c r="H11" s="10">
+      <c r="G11" s="33"/>
+      <c r="I11" s="10">
         <v>7</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
         <v>1.4966666666666668</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <f t="shared" si="3"/>
         <v>1.88</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
         <v>8</v>
       </c>
@@ -3900,27 +4064,28 @@
       <c r="F12" s="3">
         <v>0.28010000000000002</v>
       </c>
-      <c r="H12" s="10">
+      <c r="G12" s="33"/>
+      <c r="I12" s="10">
         <v>8</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
         <v>1.3117647058823529</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <f t="shared" si="3"/>
         <v>1.5561111111111112</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
         <v>9</v>
       </c>
@@ -3936,27 +4101,28 @@
       <c r="F13" s="3">
         <v>0.27339999999999998</v>
       </c>
-      <c r="H13" s="10">
+      <c r="G13" s="33"/>
+      <c r="I13" s="10">
         <v>9</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
         <v>1.1159999999999999</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <f t="shared" si="2"/>
         <v>0.21</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <f t="shared" si="3"/>
         <v>1.3019047619047619</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>10</v>
       </c>
@@ -3972,27 +4138,33 @@
       <c r="F14" s="3">
         <v>0.24740000000000001</v>
       </c>
-      <c r="H14" s="10">
+      <c r="G14" s="28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H14" s="28">
+        <v>0.22</v>
+      </c>
+      <c r="I14" s="10">
         <v>10</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <f t="shared" si="1"/>
         <v>0.91909090909090907</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <f t="shared" si="2"/>
         <v>0.23</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <f t="shared" si="3"/>
         <v>1.0756521739130436</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
         <v>11</v>
       </c>
@@ -4008,27 +4180,28 @@
       <c r="F15" s="3">
         <v>0.1883</v>
       </c>
-      <c r="H15" s="10">
+      <c r="G15" s="33"/>
+      <c r="I15" s="10">
         <v>11</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <f t="shared" si="1"/>
         <v>0.53800000000000003</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <f t="shared" si="3"/>
         <v>0.75319999999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="10">
         <v>12</v>
       </c>
@@ -4044,27 +4217,28 @@
       <c r="F16" s="3">
         <v>0.15040000000000001</v>
       </c>
-      <c r="H16" s="10">
+      <c r="G16" s="33"/>
+      <c r="I16" s="10">
         <v>12</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <f t="shared" si="1"/>
         <v>0.38285714285714284</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <f t="shared" si="3"/>
         <v>0.557037037037037</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>13</v>
       </c>
@@ -4080,27 +4254,28 @@
       <c r="F17" s="3">
         <v>0.1216</v>
       </c>
-      <c r="H17" s="10">
+      <c r="G17" s="33"/>
+      <c r="I17" s="10">
         <v>13</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <f t="shared" si="1"/>
         <v>0.29866666666666669</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <f t="shared" si="3"/>
         <v>0.40533333333333332</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="10">
         <v>14</v>
       </c>
@@ -4116,27 +4291,28 @@
       <c r="F18" s="3">
         <v>0.1119</v>
       </c>
-      <c r="H18" s="10">
+      <c r="G18" s="33"/>
+      <c r="I18" s="10">
         <v>14</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <f t="shared" si="1"/>
         <v>0.17742857142857144</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <f t="shared" si="3"/>
         <v>0.34968749999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <v>15</v>
       </c>
@@ -4152,27 +4328,28 @@
       <c r="F19" s="3">
         <v>9.4100000000000003E-2</v>
       </c>
-      <c r="H19" s="10">
+      <c r="G19" s="33"/>
+      <c r="I19" s="10">
         <v>15</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <f t="shared" si="1"/>
         <v>0.13999999999999999</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <f t="shared" si="3"/>
         <v>0.26885714285714291</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="10">
         <v>16</v>
       </c>
@@ -4188,27 +4365,28 @@
       <c r="F20" s="3">
         <v>8.2400000000000001E-2</v>
       </c>
-      <c r="H20" s="10">
+      <c r="G20" s="33"/>
+      <c r="I20" s="10">
         <v>16</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <f t="shared" si="1"/>
         <v>0.11749999999999999</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <f t="shared" si="2"/>
         <v>0.37</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <f t="shared" si="3"/>
         <v>0.2227027027027027</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>17</v>
       </c>
@@ -4224,27 +4402,28 @@
       <c r="F21" s="3">
         <v>7.0599999999999996E-2</v>
       </c>
-      <c r="H21" s="10">
+      <c r="G21" s="33"/>
+      <c r="I21" s="10">
         <v>17</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <f t="shared" si="1"/>
         <v>0.1030952380952381</v>
       </c>
-      <c r="K21" s="2">
-        <f t="shared" ref="K21:K25" si="4">E21</f>
+      <c r="L21" s="2">
+        <f t="shared" ref="L21:L25" si="4">E21</f>
         <v>0.4</v>
       </c>
-      <c r="L21" s="3">
+      <c r="M21" s="3">
         <f t="shared" si="3"/>
         <v>0.17649999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>18</v>
       </c>
@@ -4260,27 +4439,28 @@
       <c r="F22" s="3">
         <v>6.1100000000000002E-2</v>
       </c>
-      <c r="H22" s="10">
+      <c r="G22" s="33"/>
+      <c r="I22" s="10">
         <v>18</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <f t="shared" si="1"/>
         <v>8.511111111111111E-2</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <f t="shared" si="4"/>
         <v>0.43</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <f t="shared" si="3"/>
         <v>0.14209302325581397</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="10">
         <v>19</v>
       </c>
@@ -4296,27 +4476,28 @@
       <c r="F23" s="3">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="H23" s="10">
+      <c r="G23" s="33"/>
+      <c r="I23" s="10">
         <v>19</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <f t="shared" si="1"/>
         <v>7.1250000000000008E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <f t="shared" si="3"/>
         <v>0.12333333333333334</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="10">
         <v>20</v>
       </c>
@@ -4332,27 +4513,28 @@
       <c r="F24" s="3">
         <v>4.87E-2</v>
       </c>
-      <c r="H24" s="10">
+      <c r="G24" s="33"/>
+      <c r="I24" s="10">
         <v>20</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <f t="shared" si="1"/>
         <v>6.3200000000000006E-2</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <f t="shared" si="4"/>
         <v>0.48</v>
       </c>
-      <c r="L24" s="3">
+      <c r="M24" s="3">
         <f t="shared" si="3"/>
         <v>0.10145833333333333</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
         <v>21</v>
       </c>
@@ -4364,16 +4546,17 @@
       <c r="F25" s="7">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="G25" s="33"/>
+      <c r="I25" s="11">
         <v>21</v>
       </c>
-      <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6">
+      <c r="K25" s="6"/>
+      <c r="L25" s="6">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="L25" s="7">
+      <c r="M25" s="7">
         <f t="shared" si="3"/>
         <v>9.0200000000000002E-2</v>
       </c>
@@ -4381,10 +4564,10 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:F2"/>
@@ -4392,7 +4575,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J7" formula="1"/>
+    <ignoredError sqref="K7" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>